<commit_message>
I added some things to data processing
</commit_message>
<xml_diff>
--- a/REFERENCE_Post_Flight_Datasheet_Flight.xlsx
+++ b/REFERENCE_Post_Flight_Datasheet_Flight.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albi/PycharmProjects/Flight-Dynamics/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Klaas\OneDrive\Documents\GitHub\Flight-Test-B20\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_B3347193622C77B991E83D6164637CE388A2EECF" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{AA029920-8ABE-4F6E-B7E5-9704E387D608}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16260"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -350,7 +351,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
@@ -427,13 +428,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
@@ -443,9 +444,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyProtection="1">
@@ -552,6 +550,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -573,7 +574,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2"/>
+        <xdr:cNvPr id="2" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -886,25 +893,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>43171</v>
       </c>
       <c r="F3" t="s">
@@ -912,7 +919,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -924,13 +931,13 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>6</v>
       </c>
@@ -938,7 +945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -947,7 +954,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -956,7 +963,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -965,7 +972,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -974,7 +981,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -983,7 +990,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -992,7 +999,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1001,7 +1008,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1010,7 +1017,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1019,7 +1026,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1027,12 +1034,12 @@
         <v>4050</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1040,7 +1047,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1072,7 +1079,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
@@ -1101,11 +1108,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>99</v>
       </c>
       <c r="C28" s="2"/>
@@ -1131,7 +1138,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1161,7 +1168,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1191,7 +1198,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1221,7 +1228,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>5</v>
       </c>
@@ -1251,7 +1258,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>6</v>
       </c>
@@ -1281,7 +1288,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>7</v>
       </c>
@@ -1295,23 +1302,23 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>41</v>
       </c>
       <c r="E39" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -1343,7 +1350,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="s">
         <v>42</v>
       </c>
@@ -1372,7 +1379,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1386,7 +1393,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1400,7 +1407,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>3</v>
       </c>
@@ -1414,7 +1421,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4</v>
       </c>
@@ -1428,7 +1435,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>5</v>
       </c>
@@ -1442,7 +1449,7 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>6</v>
       </c>
@@ -1456,7 +1463,7 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>7</v>
       </c>
@@ -1470,17 +1477,17 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1488,7 +1495,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -1529,7 +1536,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="s">
         <v>42</v>
       </c>
@@ -1567,7 +1574,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1</v>
       </c>
@@ -1606,7 +1613,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2</v>
       </c>
@@ -1645,7 +1652,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>3</v>
       </c>
@@ -1684,7 +1691,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>4</v>
       </c>
@@ -1723,7 +1730,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>5</v>
       </c>
@@ -1762,7 +1769,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>6</v>
       </c>
@@ -1801,7 +1808,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>7</v>
       </c>
@@ -1840,23 +1847,23 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C66" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>49</v>
       </c>
       <c r="C70" s="2"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>50</v>
       </c>
@@ -1866,7 +1873,7 @@
       </c>
       <c r="H71" s="2"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>21</v>
       </c>
@@ -1907,7 +1914,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="s">
         <v>42</v>
       </c>
@@ -1945,7 +1952,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1</v>
       </c>
@@ -1984,7 +1991,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2</v>
       </c>
@@ -2023,17 +2030,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C77" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D81" t="s">
         <v>53</v>
       </c>
@@ -2044,7 +2051,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D82" t="s">
         <v>42</v>
       </c>
@@ -2055,7 +2062,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>54</v>
       </c>
@@ -2075,7 +2082,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>57</v>
       </c>
@@ -2178,7 +2185,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes to cg file
</commit_message>
<xml_diff>
--- a/REFERENCE_Post_Flight_Datasheet_Flight.xlsx
+++ b/REFERENCE_Post_Flight_Datasheet_Flight.xlsx
@@ -896,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>